<commit_message>
Reading hardware excel and assigning cols to lists
</commit_message>
<xml_diff>
--- a/Data/crypto_mining_equipment.xlsx
+++ b/Data/crypto_mining_equipment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Documents\MEng Research\crypto data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Documents\MEng Research\Crypto_IPP_model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4C46AB-0692-4232-A453-6DC69AEADBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53EB131-5E69-4D6D-B0EF-68139F190937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" xr2:uid="{54AA4049-1D40-4F51-BA56-9D8B3B076528}"/>
   </bookViews>
@@ -573,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D54727A-739B-420D-9666-27D459F44400}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -588,9 +588,10 @@
     <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>40057</v>
       </c>
@@ -634,7 +635,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>40603</v>
       </c>
@@ -655,7 +656,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2014</v>
       </c>
@@ -676,7 +677,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -699,7 +700,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>2017</v>
       </c>
@@ -724,7 +725,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>2017</v>
       </c>
@@ -748,7 +749,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43952</v>
       </c>
@@ -770,8 +771,15 @@
       <c r="G8" s="13">
         <v>11000</v>
       </c>
+      <c r="I8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="18">
+        <f>9000/15</f>
+        <v>600</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>44896</v>
       </c>
@@ -792,18 +800,7 @@
         <v>6.021E-2</v>
       </c>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="18">
-        <f>9000/15</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="18">
+      <c r="J9" s="18">
         <f>450+29+75+648+120</f>
         <v>1322</v>
       </c>

</xml_diff>

<commit_message>
Completed mining hardware specs
</commit_message>
<xml_diff>
--- a/Data/crypto_mining_equipment.xlsx
+++ b/Data/crypto_mining_equipment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Documents\MEng Research\Crypto_IPP_model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53EB131-5E69-4D6D-B0EF-68139F190937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D2EFFD-F6F9-4553-A389-323A41B24609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" xr2:uid="{54AA4049-1D40-4F51-BA56-9D8B3B076528}"/>
   </bookViews>
@@ -576,7 +576,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -789,8 +789,7 @@
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="13">
-        <f>12000/15</f>
+      <c r="D9" s="4">
         <v>800</v>
       </c>
       <c r="E9" s="5">
@@ -807,5 +806,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>